<commit_message>
updated with fan speed control
</commit_message>
<xml_diff>
--- a/Protocol_R4875g.xlsx
+++ b/Protocol_R4875g.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MJP\Documents\GitHub\CAN-BUS-control-R4875G1-with-ESPHome-and-MQTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MJP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B207BBCD-24D0-46B3-93B7-741D62DEC971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E72C21A-7CEB-4418-B40E-C5A5F6113D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
   <si>
     <t>Baud Rate 125kbps</t>
   </si>
@@ -466,16 +466,59 @@
   <si>
     <t>****0x1001117e for multible unit the message ID is following the same logic 0x1001117e 0x1002117 e0x1003117e etc…</t>
   </si>
+  <si>
+    <t>0x108182FE</t>
+  </si>
+  <si>
+    <t>0x1081827F</t>
+  </si>
+  <si>
+    <t>0x87</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>auto FAN duty</t>
+  </si>
+  <si>
+    <t>/256</t>
+  </si>
+  <si>
+    <t>0x108080FE</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>*256</t>
+  </si>
+  <si>
+    <t>Percent Duty Cycle</t>
+  </si>
+  <si>
+    <t>SET min FAN duty</t>
+  </si>
+  <si>
+    <t>Fan-speed control:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -559,6 +602,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -568,7 +617,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -646,53 +695,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -701,17 +764,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,8 +1027,8 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1018,18 +1113,18 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.5">
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="13" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:19" ht="4.5" customHeight="1">
       <c r="D7" s="4"/>
@@ -1134,12 +1229,12 @@
       <c r="G11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
       <c r="M11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1157,12 +1252,12 @@
       <c r="G12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="M12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1180,12 +1275,12 @@
       <c r="G13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
       <c r="M13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1203,12 +1298,12 @@
       <c r="G14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
       <c r="M14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1226,12 +1321,12 @@
       <c r="G15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
       <c r="M15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1249,12 +1344,12 @@
       <c r="G16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
       <c r="M16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1272,12 +1367,12 @@
       <c r="G17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
       <c r="M17" s="12" t="s">
         <v>85</v>
       </c>
@@ -1298,12 +1393,12 @@
       <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
       <c r="M18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1321,12 +1416,12 @@
       <c r="G19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="15"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
       <c r="M19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1344,12 +1439,12 @@
       <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="15"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
       <c r="M20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1370,12 +1465,12 @@
       <c r="G21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="15"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
       <c r="M21" s="5" t="s">
         <v>16</v>
       </c>
@@ -1396,12 +1491,12 @@
       <c r="G22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="15"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
       <c r="M22" s="5"/>
       <c r="N22" s="6"/>
     </row>
@@ -1454,18 +1549,18 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1">
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="13" t="s">
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="15"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
       <c r="M26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1499,12 +1594,12 @@
       <c r="G28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="15"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
       <c r="M28" s="5" t="s">
         <v>46</v>
       </c>
@@ -1526,12 +1621,12 @@
       <c r="G29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="23"/>
       <c r="M29" s="5" t="s">
         <v>46</v>
       </c>
@@ -1552,12 +1647,12 @@
       <c r="G30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="15"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="23"/>
       <c r="M30" s="5" t="s">
         <v>46</v>
       </c>
@@ -1578,12 +1673,12 @@
       <c r="G31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="15"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="23"/>
       <c r="M31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1607,12 +1702,12 @@
       <c r="G32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="15"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="23"/>
       <c r="M32" s="12" t="s">
         <v>86</v>
       </c>
@@ -1636,12 +1731,12 @@
       <c r="G33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="23"/>
       <c r="M33" s="12" t="s">
         <v>61</v>
       </c>
@@ -1748,61 +1843,61 @@
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="24" t="s">
+      <c r="D39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="19" t="s">
+      <c r="F39" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K39" s="20" t="s">
+      <c r="H39" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="16" t="s">
         <v>7</v>
       </c>
       <c r="M39" s="5"/>
-      <c r="N39" s="26" t="s">
+      <c r="N39" s="19" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="D40" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="27" t="s">
+      <c r="F40" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="23"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="26"/>
       <c r="M40" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="N40" s="25" t="s">
+      <c r="N40" s="18" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1842,26 +1937,228 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D49" s="17" t="s">
+    <row r="49" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D49" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="51" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="52" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="53" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="54" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="55" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="56" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="57" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="58" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="59" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="60" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="61" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="62" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="63" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="64" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A50" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>2</v>
+      </c>
+      <c r="G52" s="3">
+        <v>3</v>
+      </c>
+      <c r="H52" s="3">
+        <v>4</v>
+      </c>
+      <c r="I52" s="3">
+        <v>5</v>
+      </c>
+      <c r="J52" s="3">
+        <v>6</v>
+      </c>
+      <c r="K52" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D53" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="23"/>
+      <c r="M53" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="G54" s="38"/>
+      <c r="H54" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="I54" s="39"/>
+      <c r="J54" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="K54" s="41"/>
+      <c r="M54" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D56" s="30"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+    </row>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D57" s="30"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="M58" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G59" s="26"/>
+      <c r="H59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M59" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="30"/>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="30"/>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" customHeight="1">
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2799,12 +3096,26 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
+  <mergeCells count="32">
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="H32:K32"/>
     <mergeCell ref="H40:K40"/>
@@ -2813,16 +3124,11 @@
     <mergeCell ref="H21:K21"/>
     <mergeCell ref="H22:K22"/>
     <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update SET input Current Limit
</commit_message>
<xml_diff>
--- a/Protocol_R4875g.xlsx
+++ b/Protocol_R4875g.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MJP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MJP\Documents\GitHub\CAN-BUS-control-R4875G1-with-ESPHome-and-MQTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E72C21A-7CEB-4418-B40E-C5A5F6113D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE8796E-0BFE-40BB-B968-A68AFA53A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>Baud Rate 125kbps</t>
   </si>
@@ -502,16 +502,38 @@
   <si>
     <t>Fan-speed control:</t>
   </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0 disable 1 enable limit</t>
+  </si>
+  <si>
+    <t>*1024</t>
+  </si>
+  <si>
+    <t>Input Current Limit</t>
+  </si>
+  <si>
+    <t>Set AC Current Limit:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -708,103 +730,104 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1027,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1113,18 +1136,18 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.5">
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="21" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:19" ht="4.5" customHeight="1">
       <c r="D7" s="4"/>
@@ -1229,12 +1252,12 @@
       <c r="G11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="38"/>
       <c r="M11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1252,12 +1275,12 @@
       <c r="G12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="38"/>
       <c r="M12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1275,12 +1298,12 @@
       <c r="G13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="38"/>
       <c r="M13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1298,12 +1321,12 @@
       <c r="G14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
       <c r="M14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1321,12 +1344,12 @@
       <c r="G15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="23"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
       <c r="M15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1344,12 +1367,12 @@
       <c r="G16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="23"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
       <c r="M16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1367,12 +1390,12 @@
       <c r="G17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="23"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
       <c r="M17" s="12" t="s">
         <v>85</v>
       </c>
@@ -1393,12 +1416,12 @@
       <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="23"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
       <c r="M18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1416,12 +1439,12 @@
       <c r="G19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="23"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="38"/>
       <c r="M19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1439,12 +1462,12 @@
       <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="23"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
       <c r="M20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1465,12 +1488,12 @@
       <c r="G21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="23"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="38"/>
       <c r="M21" s="5" t="s">
         <v>16</v>
       </c>
@@ -1491,12 +1514,12 @@
       <c r="G22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="23"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
       <c r="M22" s="5"/>
       <c r="N22" s="6"/>
     </row>
@@ -1549,18 +1572,18 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1">
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="21" t="s">
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="23"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="38"/>
       <c r="M26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1594,12 +1617,12 @@
       <c r="G28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="38"/>
       <c r="M28" s="5" t="s">
         <v>46</v>
       </c>
@@ -1621,12 +1644,12 @@
       <c r="G29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="23"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="38"/>
       <c r="M29" s="5" t="s">
         <v>46</v>
       </c>
@@ -1647,12 +1670,12 @@
       <c r="G30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="23"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="38"/>
       <c r="M30" s="5" t="s">
         <v>46</v>
       </c>
@@ -1673,12 +1696,12 @@
       <c r="G31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="23"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="38"/>
       <c r="M31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1702,12 +1725,12 @@
       <c r="G32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="23"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="38"/>
       <c r="M32" s="12" t="s">
         <v>86</v>
       </c>
@@ -1731,12 +1754,12 @@
       <c r="G33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="27" t="s">
+      <c r="H33" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="23"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="38"/>
       <c r="M33" s="12" t="s">
         <v>61</v>
       </c>
@@ -1888,12 +1911,12 @@
       <c r="G40" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="24" t="s">
+      <c r="H40" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="26"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="35"/>
       <c r="M40" s="12" t="s">
         <v>87</v>
       </c>
@@ -1943,7 +1966,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="21" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1951,7 +1974,7 @@
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="21" t="s">
         <v>91</v>
       </c>
       <c r="D51" s="14" t="s">
@@ -2006,18 +2029,18 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D53" s="21" t="s">
+      <c r="D53" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="21" t="s">
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="23"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="38"/>
       <c r="M53" s="5" t="s">
         <v>42</v>
       </c>
@@ -2026,7 +2049,7 @@
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="21" t="s">
         <v>92</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -2035,52 +2058,52 @@
       <c r="E54" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="37" t="s">
+      <c r="F54" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G54" s="38"/>
-      <c r="H54" s="37" t="s">
+      <c r="G54" s="30"/>
+      <c r="H54" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="I54" s="39"/>
-      <c r="J54" s="40" t="s">
+      <c r="I54" s="31"/>
+      <c r="J54" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="K54" s="41"/>
-      <c r="M54" s="42" t="s">
+      <c r="K54" s="33"/>
+      <c r="M54" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="56" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D56" s="30"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D57" s="30"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="27"/>
       <c r="M58" s="5" t="s">
         <v>42</v>
       </c>
@@ -2098,10 +2121,10 @@
       <c r="E59" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F59" s="27" t="s">
+      <c r="F59" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="G59" s="26"/>
+      <c r="G59" s="35"/>
       <c r="H59" s="3" t="s">
         <v>7</v>
       </c>
@@ -2114,51 +2137,89 @@
       <c r="K59" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M59" s="43" t="s">
+      <c r="M59" s="25" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="27"/>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
+      <c r="A62" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1">
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-    </row>
-    <row r="64" spans="1:13" ht="15.75" customHeight="1"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="M63" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="49.5" customHeight="1">
+      <c r="A64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="K64" s="35"/>
+      <c r="M64" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -3096,13 +3157,18 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="F59:G59"/>
+  <mergeCells count="33">
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H33:K33"/>
     <mergeCell ref="D53:G53"/>
     <mergeCell ref="H53:K53"/>
     <mergeCell ref="H57:K57"/>
@@ -3119,16 +3185,12 @@
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="H32:K32"/>
     <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="F59:G59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>

</xml_diff>